<commit_message>
req 1 & 11
1: replace τοπ 10 και δηλωσεις with TOP 10
11: links on articles is also now on picture too
</commit_message>
<xml_diff>
--- a/ToDo/ToDo.xlsx
+++ b/ToDo/ToDo.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$H$13</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>What</t>
   </si>
@@ -135,12 +135,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -245,50 +253,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,11 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -630,13 +643,17 @@
       <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="5">
+        <v>43007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -718,7 +735,9 @@
       <c r="G6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5">
+        <v>43007</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -731,14 +750,16 @@
       <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="13"/>
-      <c r="H7" s="5"/>
+      <c r="H7" s="5">
+        <v>43007</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -954,11 +975,7 @@
       <c r="E42" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H12">
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
trying to make room for logos
</commit_message>
<xml_diff>
--- a/ToDo/ToDo.xlsx
+++ b/ToDo/ToDo.xlsx
@@ -588,7 +588,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -630,7 +630,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -654,7 +654,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -676,7 +676,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -720,7 +720,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -744,7 +744,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -832,7 +832,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Image slide - test with css and Nikos
New TODO!
</commit_message>
<xml_diff>
--- a/ToDo/ToDo.xlsx
+++ b/ToDo/ToDo.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$H$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$H$28</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>What</t>
   </si>
@@ -52,95 +52,165 @@
     <t>Θέλουμε οταν ενας χρηστης μπαίνει σε κάποιο άρθρο να υπάρχουν βελάκια(κάτω αριστερά και κάτω δεξιά) ώστε να τον πηγαίνουν στο επόμενο και στο προηγούμενο άρθρο.Αυτό θα βοηθήσει πολύ εμάς αλλά και τους χρήστες και ειδικότερα όταν θα βλέπουν το πρόγραμμα.</t>
   </si>
   <si>
-    <t>Όταν βάζουμε βίντεο δηλώσεων σε ένα άρθρο,δεν τραβάει μια εικόνα από το βίντεο ώστε να μπει φωτογραφία του άρθρου.Κόιταξε το αυτό γιατί το θέλουμε.</t>
-  </si>
-  <si>
     <t>Θέλουμε σε κάθε σελιδά μια κατηργορίας (π.χ. Γ όμιλος Α1) και κάτω από το βασικό slider να φτιαχτεί ένα πλαίσιο όπου θα χωρίζεται σε 2 μέρη.Στο πάνω μέρος θέλουμε να υπάρχουν τα άρθρα των MVP (πάντα για την συγκεκριμένη κατηγορία) και στο κάτω οι δηλώσεις.Με την ίδια λογική που στην αρχική σελίδα έχουμε αυτο :
 δες φωτο στο εμαιλ</t>
   </si>
   <si>
     <t>Κόιταξε επίσης να μπορεί ο χρήστης πατώντας την φωτό ενος άρθρου να μπαίνει κατευθείαν γιατί δεν σε αφήνει και πρέπει να πατήσει τον τίτλο.Επίσης έχουμε παρατηρήσει κάποια θέματα με την ταχύτητα.Ρίξε και εσύ μια ματιά.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>δεν θέλουμε το twitter.Μπορείς να το διώξεις.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Θέλουμε να αλλάξει στην αρχική οθόνη το "Top 10 και δηλώσεις" και να μείνει μόνο το "Top 10" </t>
+  </si>
+  <si>
+    <t>nikos</t>
+  </si>
+  <si>
+    <t>Ένα πολύ σημαντικό θέμα που μας έχει προκύψει είναι ότι η γραμματοσειρά είναι πολύ μικρή στα άρθρα(αυτή που είναι by default).Θέλουμε να κάνεις by default το 5ο heading.</t>
+  </si>
+  <si>
+    <t>Επίσης έχουμε παρατηρήσει ότι υπάρχει θέμα όταν γράφουμε σε άλλο heading μας τα βγάζει όλα σε κεφαλαία και δεν το θέλουμε.</t>
+  </si>
+  <si>
+    <t>thanasis</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Importance</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>που είναι αυτό?!?!?
+Αρχική σελίδα - 2ο Slider</t>
+  </si>
+  <si>
+    <t>τι εννοει με το 5ο heading?
+Μάλλον εννοεί τον editor</t>
+  </si>
+  <si>
+    <t>τι εννοει?
+Στα άρθρα μάλλον, όπως εμφανίζονται. Δεν ρώτησα.</t>
+  </si>
+  <si>
+    <t>Δεν θέλει τόνους - κεφαλαια κτλπ.</t>
+  </si>
+  <si>
+    <t>Δύσκολο</t>
+  </si>
+  <si>
+    <t>Θέλει να σπάσει σε 2 sliders</t>
+  </si>
+  <si>
+    <t>xmmm</t>
+  </si>
+  <si>
+    <t>Θανάση αυτό μου το έστειλαν από την sporting bet που θα γίνει χορηγός του τουρνουά. Έχουμε συμφωνήσει να βάλουμε δύο Μπάνερ δεξιά και αριστερά στα κενά του site και ένα μακρόστενο στο κέντρο τώρα πάνω από το slider η κάτω από αυτό δεν ξέρω θα το δούμε. Σε παρακαλώ στείλε μου σε τι μέγεθος θες να είναι για να του τα ζητήσω.  Από ότι είδα θέλει μέγεθος σε pixel καταλαβαίνεις τι θέλει ε;</t>
+  </si>
+  <si>
+    <t>logos</t>
+  </si>
+  <si>
+    <t>Στατιστικά site / κάτι πιο κατανοητό</t>
+  </si>
+  <si>
+    <t>Tαχύτητα / Sliders</t>
+  </si>
+  <si>
+    <t>Σε κάθε πορτοκαλί επικεφαλίδα να τον πετάει στην αντίστοιχη λίστα, βλέπε αρχικό τοπ 10.</t>
+  </si>
+  <si>
+    <t>Slider τελευταίων αγώνων να φέρνει 7 - ιδανικά της εβομάδας</t>
+  </si>
+  <si>
+    <t>GetWeeklyGames να φέρνει 7 παιχνίδια</t>
+  </si>
+  <si>
+    <t>Βαθμολογία - Νίκες + Ήττες + Μηδενισμοί + Πόντοι + Διαφορά Πόντων</t>
+  </si>
+  <si>
+    <t>Στα datatables να είναι σε μια σελίδα, π.χ. 3η από 10 να τον γυρνάει στην ίδια σελίδα…</t>
+  </si>
+  <si>
+    <t>Οι δηλώσεις --- είναι max 7! Να φαίνονται.</t>
+  </si>
+  <si>
+    <t>MVP - Δεν έχει βίντεο! Να μην είναι υποχρεωτικό!</t>
+  </si>
+  <si>
+    <t>MVP - να ομορφύνει designata</t>
+  </si>
+  <si>
+    <t>"Δείτε λίστα με όλα τα νέα" να γίνει pagging παρόμοιο με τα datatables</t>
   </si>
   <si>
     <t>Τέλος,θέλουμε να μπει ένα counter στο τέλος τέλος της αρχικής που θα έχει 3 πλαίσια.
 Πλαίσιο 1 : Συνολικοί χρήστες που έχουν επισκεφτεί το site = X
 Πλαίσιο 2 : Συνολικοί χρήστες που έχουν επισκεφτεί το site τον τελευταίο μήνα = Y
-Πλαίσιο 3 : Πόσοι χρήστες βρίκονται αυτή τη στιγμή στην σελίδα (εγγεγραμένοι και όχι).</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Finished</t>
-  </si>
-  <si>
-    <t>δεν θέλουμε το twitter.Μπορείς να το διώξεις.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Θέλουμε να αλλάξει στην αρχική οθόνη το "Top 10 και δηλώσεις" και να μείνει μόνο το "Top 10" </t>
-  </si>
-  <si>
-    <t>nikos</t>
-  </si>
-  <si>
-    <t>Ένα πολύ σημαντικό θέμα που μας έχει προκύψει είναι ότι η γραμματοσειρά είναι πολύ μικρή στα άρθρα(αυτή που είναι by default).Θέλουμε να κάνεις by default το 5ο heading.</t>
-  </si>
-  <si>
-    <t>Επίσης έχουμε παρατηρήσει ότι υπάρχει θέμα όταν γράφουμε σε άλλο heading μας τα βγάζει όλα σε κεφαλαία και δεν το θέλουμε.</t>
-  </si>
-  <si>
-    <t>thanasis</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Importance</t>
-  </si>
-  <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t>που είναι αυτό?!?!?
-Αρχική σελίδα - 2ο Slider</t>
-  </si>
-  <si>
-    <t>τι εννοει με το 5ο heading?
-Μάλλον εννοεί τον editor</t>
-  </si>
-  <si>
-    <t>τι εννοει?
-Στα άρθρα μάλλον, όπως εμφανίζονται. Δεν ρώτησα.</t>
-  </si>
-  <si>
-    <t>Δεν θέλει τόνους - κεφαλαια κτλπ.</t>
-  </si>
-  <si>
-    <t>Δύσκολο</t>
-  </si>
-  <si>
-    <t>Θέλει να σπάσει σε 2 sliders</t>
-  </si>
-  <si>
-    <t>xmmm</t>
-  </si>
-  <si>
-    <t>Θανάση αυτό μου το έστειλαν από την sporting bet που θα γίνει χορηγός του τουρνουά. Έχουμε συμφωνήσει να βάλουμε δύο Μπάνερ δεξιά και αριστερά στα κενά του site και ένα μακρόστενο στο κέντρο τώρα πάνω από το slider η κάτω από αυτό δεν ξέρω θα το δούμε. Σε παρακαλώ στείλε μου σε τι μέγεθος θες να είναι για να του τα ζητήσω.  Από ότι είδα θέλει μέγεθος σε pixel καταλαβαίνεις τι θέλει ε;</t>
-  </si>
-  <si>
-    <t>logos</t>
+Πλαίσιο 3 : Πόσοι χρήστες βρίκονται αυτή τη στιγμή στην σελίδα (εγγεγραμένοι και όχι).
+Βλέπε Whiteart.gr, έχει ένα κίτρινο counter με μεγάλα κουτιά</t>
+  </si>
+  <si>
+    <t>Eurohoops facebook - Δεν έχει εικόνες.</t>
+  </si>
+  <si>
+    <t>Widget - πλαίσιο - άρθρα -&gt; ένα πλαίσιο να μην είναι αχνό.</t>
+  </si>
+  <si>
+    <t>Στα άρθρα - βλέπε αρχική - αν δεν έχει στην περίληψη κάτι να τραβήξει από το κείμενο να μην φαίνεται άδειο.</t>
+  </si>
+  <si>
+    <t>Στις λιστες όταν πατάει την εικόνα δεν τον πάει στο άρθρο.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Όταν βάζουμε βίντεο δηλώσεων σε ένα άρθρο,δεν τραβάει μια εικόνα από το βίντεο ώστε να μπει φωτογραφία του άρθρου.Κόιταξε το αυτό γιατί το θέλουμε.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Μόνο αν είναι ΔΗΛΩΣΗ ή TOP 10!</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -237,48 +307,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,10 +630,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A11" activeCellId="4" sqref="A2:A3 A6 A7 A10 A11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -580,13 +652,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -598,13 +670,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -616,19 +688,19 @@
         <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H2" s="5">
         <v>43007</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -640,10 +712,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="12">
@@ -662,17 +734,17 @@
         <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -684,15 +756,17 @@
         <v>6</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="H5" s="5">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -707,16 +781,16 @@
         <v>4</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H6" s="5">
         <v>43007</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -731,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="5">
@@ -753,14 +827,14 @@
         <v>8</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>9</v>
       </c>
@@ -772,17 +846,17 @@
         <v>7</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>10</v>
       </c>
@@ -794,17 +868,19 @@
         <v>7</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H10" s="5">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>11</v>
       </c>
@@ -816,17 +892,17 @@
         <v>7</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="5">
         <v>43007</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>12</v>
       </c>
@@ -838,13 +914,13 @@
         <v>7</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -857,70 +933,190 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="9"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E14" s="13"/>
+      <c r="A14" s="3">
+        <v>14</v>
+      </c>
+      <c r="B14" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E15" s="13"/>
+      <c r="A15" s="3">
+        <v>15</v>
+      </c>
+      <c r="B15" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>16</v>
+      </c>
+      <c r="B16" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>17</v>
+      </c>
+      <c r="B17" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>18</v>
+      </c>
+      <c r="B18" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>19</v>
+      </c>
+      <c r="B19" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>20</v>
+      </c>
+      <c r="B20" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>21</v>
+      </c>
+      <c r="B21" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>23</v>
+      </c>
+      <c r="B23" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>24</v>
+      </c>
+      <c r="B24" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>25</v>
+      </c>
+      <c r="B25" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>26</v>
+      </c>
+      <c r="B26" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>27</v>
+      </c>
+      <c r="B27" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>28</v>
+      </c>
+      <c r="B28" s="15">
+        <v>43011</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E29" s="13"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E31" s="13"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.3">
@@ -954,7 +1150,11 @@
       <c r="E42" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H13"/>
+  <autoFilter ref="A1:H28">
+    <filterColumn colId="7">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Done: 9, 16, 19, 29
</commit_message>
<xml_diff>
--- a/ToDo/ToDo.xlsx
+++ b/ToDo/ToDo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>What</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Working on it.</t>
+  </si>
+  <si>
+    <t>Λίστα με ενεργούς παίχτες</t>
   </si>
 </sst>
 </file>
@@ -313,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -347,6 +350,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -647,7 +653,7 @@
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -851,7 +857,9 @@
       <c r="G9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4">
+        <v>43017</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -989,7 +997,9 @@
       <c r="G16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4">
+        <v>43017</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1043,7 +1053,9 @@
       <c r="G19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="4">
+        <v>43017</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1198,7 +1210,18 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A29" s="3">
+        <v>29</v>
+      </c>
+      <c r="B29" s="12">
+        <v>43017</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="12">
+        <v>43017</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H28"/>

</xml_diff>

<commit_message>
todo excel change in filters... not an actual change...
</commit_message>
<xml_diff>
--- a/ToDo/ToDo.xlsx
+++ b/ToDo/ToDo.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$H$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$H$29</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -348,11 +348,11 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,10 +634,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -648,7 +649,7 @@
     <col min="4" max="4" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="102.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -679,7 +680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -703,7 +704,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -747,7 +748,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -769,7 +770,7 @@
         <v>43009</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -793,7 +794,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -837,7 +838,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -861,7 +862,7 @@
         <v>43017</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -885,7 +886,7 @@
         <v>43009</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -929,7 +930,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -981,7 +982,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1019,7 +1020,7 @@
       </c>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1037,7 +1038,7 @@
         <v>43015</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1073,7 +1074,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>43015</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1141,7 +1142,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1191,7 +1192,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1209,22 +1210,26 @@
         <v>43015</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>29</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="11">
         <v>43017</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="11">
         <v>43017</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H28"/>
+  <autoFilter ref="A1:H29">
+    <filterColumn colId="7">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
To do list updated with ticket type!
</commit_message>
<xml_diff>
--- a/ToDo/ToDo.xlsx
+++ b/ToDo/ToDo.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$H$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Φύλλο1!$A$1:$I$40</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
   <si>
     <t>What</t>
   </si>
@@ -257,17 +257,43 @@
   <si>
     <t>Στατιστικά site / κάτι πιο κατανοητό από το google statistics</t>
   </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Μικρή διόρθωση</t>
+  </si>
+  <si>
+    <t>Διόρθωση</t>
+  </si>
+  <si>
+    <t>Αλλαγή/Προσθήκη</t>
+  </si>
+  <si>
+    <t>Διόρθωση/Αλλαγή</t>
+  </si>
+  <si>
+    <t>Διορθώσεις/Αλλαγές</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -381,40 +407,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -700,10 +729,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -711,15 +740,16 @@
     <col min="1" max="1" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="102.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="20.140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -744,8 +774,11 @@
       <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -768,8 +801,11 @@
       <c r="H2" s="4">
         <v>43007</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -790,8 +826,11 @@
       <c r="H3" s="10">
         <v>43007</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -814,8 +853,11 @@
       <c r="H4" s="4">
         <v>43019</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -836,8 +878,11 @@
       <c r="H5" s="4">
         <v>43009</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -860,8 +905,11 @@
       <c r="H6" s="4">
         <v>43007</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -882,8 +930,11 @@
       <c r="H7" s="4">
         <v>43007</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -906,8 +957,11 @@
       <c r="H8" s="4">
         <v>43019</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -930,8 +984,11 @@
       <c r="H9" s="4">
         <v>43017</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -954,8 +1011,11 @@
       <c r="H10" s="4">
         <v>43009</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -976,8 +1036,11 @@
       <c r="H11" s="4">
         <v>43007</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="I11" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -998,8 +1061,11 @@
         <v>50</v>
       </c>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -1018,8 +1084,11 @@
       <c r="H13" s="4">
         <v>43015</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -1034,8 +1103,11 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I14" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -1050,8 +1122,11 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1070,8 +1145,11 @@
       <c r="H16" s="4">
         <v>43017</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I16" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1088,8 +1166,11 @@
         <v>46</v>
       </c>
       <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1106,8 +1187,11 @@
       <c r="H18" s="4">
         <v>43015</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1126,8 +1210,11 @@
       <c r="H19" s="4">
         <v>43017</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I19" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -1142,8 +1229,11 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1160,8 +1250,11 @@
       <c r="H21" s="4">
         <v>43015</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1178,8 +1271,11 @@
       <c r="H22" s="4">
         <v>43015</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I22" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1193,9 +1289,14 @@
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="4">
+        <v>43031</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1212,8 +1313,11 @@
       <c r="H24" s="4">
         <v>43025</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1230,8 +1334,11 @@
       <c r="H25" s="4">
         <v>43015</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I25" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>26</v>
       </c>
@@ -1248,8 +1355,11 @@
       <c r="H26" s="4">
         <v>43029</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1268,8 +1378,11 @@
       <c r="H27" s="4">
         <v>43020</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1286,8 +1399,11 @@
       <c r="H28" s="4">
         <v>43015</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1304,8 +1420,11 @@
       <c r="H29" s="4">
         <v>43017</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I29" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1320,8 +1439,11 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I30" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1338,8 +1460,11 @@
         <v>60</v>
       </c>
       <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I31" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1356,8 +1481,11 @@
       <c r="H32" s="4">
         <v>43029</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>33</v>
       </c>
@@ -1376,8 +1504,11 @@
       <c r="H33" s="4">
         <v>43025</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>34</v>
       </c>
@@ -1394,8 +1525,11 @@
       <c r="H34" s="4">
         <v>43025</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1414,8 +1548,11 @@
       <c r="H35" s="4">
         <v>43025</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1432,8 +1569,11 @@
       <c r="H36" s="4">
         <v>43025</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1452,8 +1592,11 @@
       <c r="H37" s="4">
         <v>43025</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I37" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1468,8 +1611,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>39</v>
       </c>
@@ -1486,8 +1632,11 @@
       <c r="H39" s="4">
         <v>43027</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="I39" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -1504,11 +1653,16 @@
       <c r="H40" s="4">
         <v>43029</v>
       </c>
+      <c r="I40" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H40">
-    <filterColumn colId="7">
-      <filters blank="1"/>
+  <autoFilter ref="A1:I40">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Αλλαγή/Προσθήκη"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Eikones apo to live kai dokimes gia slides
</commit_message>
<xml_diff>
--- a/ToDo/ToDo.xlsx
+++ b/ToDo/ToDo.xlsx
@@ -734,8 +734,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -833,7 +833,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -941,7 +941,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -971,7 +971,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1466,7 +1466,9 @@
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4">
+        <v>43032</v>
+      </c>
       <c r="I30" s="4" t="s">
         <v>72</v>
       </c>
@@ -1699,10 +1701,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I40">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Αλλαγή/Προσθήκη"/>
-      </filters>
+    <filterColumn colId="7">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>